<commit_message>
Moved the Network to NetworkData transfer into the NetworkData class.
</commit_message>
<xml_diff>
--- a/experiments/results/results.xlsx
+++ b/experiments/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VU\Code\SubFlow\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6789872F-84AB-4668-869A-E45FDDEF1282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205BB431-F0D7-4C15-BC36-68C10265C8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="6675" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -165,6 +165,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color auto="1"/>
@@ -218,19 +233,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -276,6 +278,21 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -294,13 +311,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -310,15 +323,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,7 +619,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -734,30 +751,30 @@
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="14">
+      <c r="A12" s="12">
         <v>100</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="15">
         <f xml:space="preserve"> S8 * A12 / 100</f>
         <v>546.5078125</v>
       </c>
@@ -779,10 +796,10 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="15">
+      <c r="A13" s="13">
         <v>90</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="16">
         <f xml:space="preserve"> S8 * A13 / 100</f>
         <v>491.85703124999998</v>
       </c>
@@ -804,10 +821,10 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="15">
+      <c r="A14" s="13">
         <v>80</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="16">
         <f xml:space="preserve"> S8 * A14 / 100</f>
         <v>437.20625000000001</v>
       </c>
@@ -829,10 +846,10 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="15">
+      <c r="A15" s="13">
         <v>70</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="16">
         <f xml:space="preserve"> S8 * A15 / 100</f>
         <v>382.55546874999999</v>
       </c>
@@ -854,10 +871,10 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="15">
+      <c r="A16" s="13">
         <v>60</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="16">
         <f xml:space="preserve"> S8 * A16 / 100</f>
         <v>327.90468750000002</v>
       </c>
@@ -879,10 +896,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="15">
+      <c r="A17" s="13">
         <v>50</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="16">
         <f xml:space="preserve"> S8 * A17 / 100</f>
         <v>273.25390625</v>
       </c>
@@ -904,10 +921,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="15">
+      <c r="A18" s="13">
         <v>40</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="16">
         <f xml:space="preserve"> S8 * A18 / 100</f>
         <v>218.60312500000001</v>
       </c>
@@ -929,10 +946,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="15">
+      <c r="A19" s="13">
         <v>30</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="16">
         <f xml:space="preserve"> S8 * A19 / 100</f>
         <v>163.95234375000001</v>
       </c>
@@ -954,10 +971,10 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="15">
+      <c r="A20" s="13">
         <v>20</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="16">
         <f xml:space="preserve"> S8 * A20 / 100</f>
         <v>109.3015625</v>
       </c>
@@ -979,10 +996,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="16">
+      <c r="A21" s="14">
         <v>10</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="17">
         <f xml:space="preserve"> S8 * A21 / 100</f>
         <v>54.650781250000001</v>
       </c>

</xml_diff>

<commit_message>
Fixed displaying of accuracy in results table.
</commit_message>
<xml_diff>
--- a/experiments/results/results.xlsx
+++ b/experiments/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VU\Code\SubFlow\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205BB431-F0D7-4C15-BC36-68C10265C8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C4105B-CE46-4133-B26C-37EA928B17F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="6675" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -306,14 +306,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -336,6 +332,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,7 +619,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -635,17 +635,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="R1" s="6" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="R1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="6"/>
+      <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -658,7 +658,7 @@
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="R2" s="1" t="s">
@@ -751,273 +751,233 @@
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="12">
+      <c r="A12" s="8">
         <v>100</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="11">
         <f xml:space="preserve"> S8 * A12 / 100</f>
         <v>546.5078125</v>
       </c>
-      <c r="C12" s="4">
-        <f xml:space="preserve"> 0.989000022411346 * 100</f>
-        <v>98.900002241134601</v>
-      </c>
-      <c r="D12" s="4">
-        <f xml:space="preserve"> 0.9825000166893 * 100</f>
-        <v>98.250001668929997</v>
-      </c>
-      <c r="E12" s="4">
-        <f xml:space="preserve"> 0.989499986171722 * 100</f>
-        <v>98.949998617172199</v>
-      </c>
-      <c r="F12" s="7">
-        <f xml:space="preserve"> 0.991800010204315 * 100</f>
-        <v>99.18000102043149</v>
+      <c r="C12" s="16">
+        <v>0.98900002241134599</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0.98250001668929998</v>
+      </c>
+      <c r="E12" s="16">
+        <v>0.98949998617172197</v>
+      </c>
+      <c r="F12" s="17">
+        <v>0.99180001020431496</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="13">
+      <c r="A13" s="9">
         <v>90</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="12">
         <f xml:space="preserve"> S8 * A13 / 100</f>
         <v>491.85703124999998</v>
       </c>
-      <c r="C13" s="4">
-        <f xml:space="preserve"> 0.983699977397918 * 100</f>
-        <v>98.369997739791799</v>
-      </c>
-      <c r="D13" s="4">
-        <f xml:space="preserve"> 0.988200008869171 * 100</f>
-        <v>98.8200008869171</v>
-      </c>
-      <c r="E13" s="4">
-        <f xml:space="preserve"> 0.985700011253356 * 100</f>
-        <v>98.570001125335608</v>
-      </c>
-      <c r="F13" s="7">
-        <f xml:space="preserve"> 0.988300025463104 * 100</f>
-        <v>98.830002546310396</v>
+      <c r="C13" s="16">
+        <v>0.98369997739791804</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0.98820000886917103</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0.98570001125335605</v>
+      </c>
+      <c r="F13" s="17">
+        <v>0.98830002546310403</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="13">
+      <c r="A14" s="9">
         <v>80</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="12">
         <f xml:space="preserve"> S8 * A14 / 100</f>
         <v>437.20625000000001</v>
       </c>
-      <c r="C14" s="4">
-        <f xml:space="preserve"> 0.975199997425079 * 100</f>
-        <v>97.519999742507906</v>
-      </c>
-      <c r="D14" s="4">
-        <f xml:space="preserve"> 0.985099971294403 * 100</f>
-        <v>98.509997129440293</v>
-      </c>
-      <c r="E14" s="4">
-        <f xml:space="preserve"> 0.990100026130676 * 100</f>
-        <v>99.010002613067599</v>
-      </c>
-      <c r="F14" s="7">
-        <f xml:space="preserve"> 0.989600002765655 * 100</f>
-        <v>98.960000276565495</v>
+      <c r="C14" s="16">
+        <v>0.97519999742507901</v>
+      </c>
+      <c r="D14" s="16">
+        <v>0.98509997129440297</v>
+      </c>
+      <c r="E14" s="16">
+        <v>0.99010002613067605</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0.98960000276565496</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="13">
+      <c r="A15" s="9">
         <v>70</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="12">
         <f xml:space="preserve"> S8 * A15 / 100</f>
         <v>382.55546874999999</v>
       </c>
-      <c r="C15" s="4">
-        <f xml:space="preserve"> 0.963800013065338 * 100</f>
-        <v>96.380001306533799</v>
-      </c>
-      <c r="D15" s="4">
-        <f xml:space="preserve"> 0.98360002040863 * 100</f>
-        <v>98.360002040863009</v>
-      </c>
-      <c r="E15" s="4">
-        <f xml:space="preserve"> 0.987800002098083 * 100</f>
-        <v>98.780000209808307</v>
-      </c>
-      <c r="F15" s="7">
-        <f xml:space="preserve"> 0.986000001430511 * 100</f>
-        <v>98.600000143051105</v>
+      <c r="C15" s="16">
+        <v>0.96380001306533802</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0.98360002040863004</v>
+      </c>
+      <c r="E15" s="16">
+        <v>0.98780000209808305</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.98600000143051103</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="13">
+      <c r="A16" s="9">
         <v>60</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="12">
         <f xml:space="preserve"> S8 * A16 / 100</f>
         <v>327.90468750000002</v>
       </c>
-      <c r="C16" s="4">
-        <f xml:space="preserve"> 0.952700018882751 * 100</f>
-        <v>95.270001888275104</v>
-      </c>
-      <c r="D16" s="4">
-        <f xml:space="preserve"> 0.983299970626831 * 100</f>
-        <v>98.329997062683105</v>
-      </c>
-      <c r="E16" s="4">
-        <f xml:space="preserve"> 0.98769998550415 * 100</f>
-        <v>98.769998550414996</v>
-      </c>
-      <c r="F16" s="7">
-        <f xml:space="preserve"> 0.990899980068206 * 100</f>
-        <v>99.089998006820608</v>
+      <c r="C16" s="16">
+        <v>0.95270001888275102</v>
+      </c>
+      <c r="D16" s="16">
+        <v>0.98329997062683105</v>
+      </c>
+      <c r="E16" s="16">
+        <v>0.98769998550414995</v>
+      </c>
+      <c r="F16" s="17">
+        <v>0.99089998006820601</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="13">
+      <c r="A17" s="9">
         <v>50</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="12">
         <f xml:space="preserve"> S8 * A17 / 100</f>
         <v>273.25390625</v>
       </c>
-      <c r="C17" s="4">
-        <f xml:space="preserve"> 0.919900000095367 * 100</f>
-        <v>91.990000009536701</v>
-      </c>
-      <c r="D17" s="4">
-        <f xml:space="preserve"> 0.985400021076202 * 100</f>
-        <v>98.540002107620197</v>
-      </c>
-      <c r="E17" s="4">
-        <f xml:space="preserve"> 0.987900018692016 * 100</f>
-        <v>98.790001869201603</v>
-      </c>
-      <c r="F17" s="7">
-        <f xml:space="preserve"> 0.989000022411346 * 100</f>
-        <v>98.900002241134601</v>
+      <c r="C17" s="16">
+        <v>0.91990000009536699</v>
+      </c>
+      <c r="D17" s="16">
+        <v>0.98540002107620195</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0.98790001869201605</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0.98900002241134599</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="13">
+      <c r="A18" s="9">
         <v>40</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="12">
         <f xml:space="preserve"> S8 * A18 / 100</f>
         <v>218.60312500000001</v>
       </c>
-      <c r="C18" s="4">
-        <f xml:space="preserve"> 0.751900017261505 * 100</f>
-        <v>75.190001726150498</v>
-      </c>
-      <c r="D18" s="4">
-        <f xml:space="preserve"> 0.984200000762939 * 100</f>
-        <v>98.420000076293903</v>
-      </c>
-      <c r="E18" s="4">
-        <f xml:space="preserve"> 0.98549997806549 * 100</f>
-        <v>98.549997806549001</v>
-      </c>
-      <c r="F18" s="7">
-        <f xml:space="preserve"> 0.987299978733062 * 100</f>
-        <v>98.729997873306203</v>
+      <c r="C18" s="16">
+        <v>0.75190001726150502</v>
+      </c>
+      <c r="D18" s="16">
+        <v>0.98420000076293901</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0.98549997806548995</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0.98729997873306197</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="13">
+      <c r="A19" s="9">
         <v>30</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="12">
         <f xml:space="preserve"> S8 * A19 / 100</f>
         <v>163.95234375000001</v>
       </c>
-      <c r="C19" s="4">
-        <f xml:space="preserve"> 0.447100013494491 * 100</f>
-        <v>44.710001349449101</v>
-      </c>
-      <c r="D19" s="4">
-        <f xml:space="preserve"> 0.983099997043609 * 100</f>
-        <v>98.309999704360891</v>
-      </c>
-      <c r="E19" s="4">
-        <f xml:space="preserve"> 0.986199975013732 * 100</f>
-        <v>98.619997501373206</v>
-      </c>
-      <c r="F19" s="7">
-        <f xml:space="preserve"> 0.985300004482269 * 100</f>
-        <v>98.5300004482269</v>
+      <c r="C19" s="16">
+        <v>0.44710001349449102</v>
+      </c>
+      <c r="D19" s="16">
+        <v>0.98309999704360895</v>
+      </c>
+      <c r="E19" s="16">
+        <v>0.98619997501373202</v>
+      </c>
+      <c r="F19" s="17">
+        <v>0.98530000448226895</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="13">
+      <c r="A20" s="9">
         <v>20</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="12">
         <f xml:space="preserve"> S8 * A20 / 100</f>
         <v>109.3015625</v>
       </c>
-      <c r="C20" s="4">
-        <f xml:space="preserve"> 0.100400000810623 * 100</f>
-        <v>10.040000081062301</v>
-      </c>
-      <c r="D20" s="4">
-        <f xml:space="preserve"> 0.977100014686584 * 100</f>
-        <v>97.710001468658405</v>
-      </c>
-      <c r="E20" s="4">
-        <f xml:space="preserve"> 0.980599999427795 * 100</f>
-        <v>98.059999942779498</v>
-      </c>
-      <c r="F20" s="7">
-        <f xml:space="preserve"> 0.984000027179718 * 100</f>
-        <v>98.400002717971802</v>
+      <c r="C20" s="16">
+        <v>0.100400000810623</v>
+      </c>
+      <c r="D20" s="16">
+        <v>0.97710001468658403</v>
+      </c>
+      <c r="E20" s="16">
+        <v>0.98059999942779497</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0.98400002717971802</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="14">
+      <c r="A21" s="10">
         <v>10</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="13">
         <f xml:space="preserve"> S8 * A21 / 100</f>
         <v>54.650781250000001</v>
       </c>
-      <c r="C21" s="8">
-        <f xml:space="preserve"> 0.09740000218153 * 100</f>
-        <v>9.7400002181529999</v>
-      </c>
-      <c r="D21" s="8">
-        <f xml:space="preserve"> 0.963100016117095 * 100</f>
-        <v>96.310001611709495</v>
-      </c>
-      <c r="E21" s="8">
-        <f xml:space="preserve"> 0.974900007247924 * 100</f>
-        <v>97.490000724792409</v>
-      </c>
-      <c r="F21" s="9">
-        <f xml:space="preserve"> 0.977900028228759 * 100</f>
-        <v>97.790002822875906</v>
+      <c r="C21" s="18">
+        <v>9.7400002181529999E-2</v>
+      </c>
+      <c r="D21" s="18">
+        <v>0.96310001611709495</v>
+      </c>
+      <c r="E21" s="18">
+        <v>0.97490000724792403</v>
+      </c>
+      <c r="F21" s="19">
+        <v>0.97790002822875899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved compression experiment evaluation.
</commit_message>
<xml_diff>
--- a/experiments/results/results.xlsx
+++ b/experiments/results/results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VU\Code\SubFlow\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C4105B-CE46-4133-B26C-37EA928B17F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C57E1C-CA27-4537-9B5E-089D0A4D4CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="6675" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="6675" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline" sheetId="1" r:id="rId1"/>
+    <sheet name="Compression (Progressive)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>Baseline</t>
   </si>
@@ -99,6 +100,30 @@
   <si>
     <t>Memory in KB</t>
   </si>
+  <si>
+    <t>Compression Rate</t>
+  </si>
+  <si>
+    <t>Relative to base</t>
+  </si>
+  <si>
+    <t>Relative to previous</t>
+  </si>
+  <si>
+    <t>Overall compression</t>
+  </si>
+  <si>
+    <t>Memory Size (Bytes)</t>
+  </si>
+  <si>
+    <t>Memory Size (MB)</t>
+  </si>
+  <si>
+    <t>% of non-zero</t>
+  </si>
+  <si>
+    <t>Individual compression</t>
+  </si>
 </sst>
 </file>
 
@@ -132,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -233,6 +258,57 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -301,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -310,13 +386,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -327,8 +407,8 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -336,6 +416,74 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -751,232 +899,232 @@
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="8">
+      <c r="A12" s="10">
         <v>100</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="13">
         <f xml:space="preserve"> S8 * A12 / 100</f>
         <v>546.5078125</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="18">
         <v>0.98900002241134599</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="18">
         <v>0.98250001668929998</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="18">
         <v>0.98949998617172197</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="19">
         <v>0.99180001020431496</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="9">
+      <c r="A13" s="11">
         <v>90</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="14">
         <f xml:space="preserve"> S8 * A13 / 100</f>
         <v>491.85703124999998</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="18">
         <v>0.98369997739791804</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="18">
         <v>0.98820000886917103</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="18">
         <v>0.98570001125335605</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="19">
         <v>0.98830002546310403</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
+      <c r="A14" s="11">
         <v>80</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="14">
         <f xml:space="preserve"> S8 * A14 / 100</f>
         <v>437.20625000000001</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="18">
         <v>0.97519999742507901</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="18">
         <v>0.98509997129440297</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="18">
         <v>0.99010002613067605</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="19">
         <v>0.98960000276565496</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="9">
+      <c r="A15" s="11">
         <v>70</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="14">
         <f xml:space="preserve"> S8 * A15 / 100</f>
         <v>382.55546874999999</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="18">
         <v>0.96380001306533802</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="18">
         <v>0.98360002040863004</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="18">
         <v>0.98780000209808305</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="19">
         <v>0.98600000143051103</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="9">
+      <c r="A16" s="11">
         <v>60</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="14">
         <f xml:space="preserve"> S8 * A16 / 100</f>
         <v>327.90468750000002</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="18">
         <v>0.95270001888275102</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="18">
         <v>0.98329997062683105</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="18">
         <v>0.98769998550414995</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="19">
         <v>0.99089998006820601</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="9">
+      <c r="A17" s="11">
         <v>50</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="14">
         <f xml:space="preserve"> S8 * A17 / 100</f>
         <v>273.25390625</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="18">
         <v>0.91990000009536699</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="18">
         <v>0.98540002107620195</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="18">
         <v>0.98790001869201605</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="19">
         <v>0.98900002241134599</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="9">
+      <c r="A18" s="11">
         <v>40</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="14">
         <f xml:space="preserve"> S8 * A18 / 100</f>
         <v>218.60312500000001</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="18">
         <v>0.75190001726150502</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="18">
         <v>0.98420000076293901</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="18">
         <v>0.98549997806548995</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="19">
         <v>0.98729997873306197</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="9">
+      <c r="A19" s="11">
         <v>30</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="14">
         <f xml:space="preserve"> S8 * A19 / 100</f>
         <v>163.95234375000001</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="18">
         <v>0.44710001349449102</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="18">
         <v>0.98309999704360895</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="18">
         <v>0.98619997501373202</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="19">
         <v>0.98530000448226895</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="9">
+      <c r="A20" s="11">
         <v>20</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="14">
         <f xml:space="preserve"> S8 * A20 / 100</f>
         <v>109.3015625</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="18">
         <v>0.100400000810623</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="18">
         <v>0.97710001468658403</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="18">
         <v>0.98059999942779497</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="19">
         <v>0.98400002717971802</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="10">
+      <c r="A21" s="12">
         <v>10</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="15">
         <f xml:space="preserve"> S8 * A21 / 100</f>
         <v>54.650781250000001</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="20">
         <v>9.7400002181529999E-2</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="20">
         <v>0.96310001611709495</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="20">
         <v>0.97490000724792403</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="21">
         <v>0.97790002822875899</v>
       </c>
     </row>
@@ -988,4 +1136,2196 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A60F5E-7815-43C4-9A13-703702D5ED07}">
+  <dimension ref="A3:X41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z42" sqref="Z42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="14" max="14" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+    </row>
+    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+    </row>
+    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="35"/>
+      <c r="X7" s="36"/>
+    </row>
+    <row r="8" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="6">
+        <v>10</v>
+      </c>
+      <c r="D8" s="47">
+        <v>20</v>
+      </c>
+      <c r="E8" s="47">
+        <v>30</v>
+      </c>
+      <c r="F8" s="47">
+        <v>40</v>
+      </c>
+      <c r="G8" s="47">
+        <v>50</v>
+      </c>
+      <c r="H8" s="47">
+        <v>60</v>
+      </c>
+      <c r="I8" s="47">
+        <v>70</v>
+      </c>
+      <c r="J8" s="47">
+        <v>80</v>
+      </c>
+      <c r="K8" s="27">
+        <v>90</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="47">
+        <v>20</v>
+      </c>
+      <c r="R8" s="47">
+        <v>30</v>
+      </c>
+      <c r="S8" s="47">
+        <v>40</v>
+      </c>
+      <c r="T8" s="47">
+        <v>50</v>
+      </c>
+      <c r="U8" s="47">
+        <v>60</v>
+      </c>
+      <c r="V8" s="47">
+        <v>70</v>
+      </c>
+      <c r="W8" s="47">
+        <v>80</v>
+      </c>
+      <c r="X8" s="27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A9" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="25">
+        <v>100</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.99180000999999995</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.99180000999999995</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.99180000999999995</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.99180000999999995</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.99180000999999995</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.99180000999999995</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.99180000999999995</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.99180000999999995</v>
+      </c>
+      <c r="K9" s="41">
+        <v>0.99180000999999995</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="25">
+        <v>100</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="X9" s="41">
+        <v>0.99180001020431519</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A10" s="32"/>
+      <c r="B10" s="26">
+        <v>90</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.98830002500000003</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.98830002500000003</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.98830002500000003</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.98830002500000003</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.98830002500000003</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.98849999899999996</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.98909997900000002</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.99110001299999995</v>
+      </c>
+      <c r="K10" s="41">
+        <v>0.99080002300000003</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="26">
+        <v>90</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0.98830002546310425</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0.98820000886917114</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0.98869997262954712</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0.99000000953674316</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0.99049997329711914</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0.99070000648498535</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0.99029999971389771</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0.98909997940063477</v>
+      </c>
+      <c r="X10" s="41">
+        <v>0.9879000186920166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A11" s="32"/>
+      <c r="B11" s="26">
+        <v>80</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.98960000299999995</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.98960000299999995</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.98960000299999995</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.98960000299999995</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.98960000299999995</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.98960000299999995</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.98970001900000004</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.98839998200000001</v>
+      </c>
+      <c r="K11" s="41">
+        <v>0.98739999499999997</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="26">
+        <v>80</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0.98960000276565552</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0.98930001258850098</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0.98930001258850098</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0.98940002918243408</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0.98799997568130493</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0.98739999532699585</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0.98669999837875366</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0.98530000448226929</v>
+      </c>
+      <c r="X11" s="41">
+        <v>0.98329997062683105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A12" s="32"/>
+      <c r="B12" s="26">
+        <v>70</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.98600000099999996</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.98600000099999996</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.98600000099999996</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.98600000099999996</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.98600000099999996</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.98610001800000002</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.98629999199999996</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.98509997100000002</v>
+      </c>
+      <c r="K12" s="41">
+        <v>0.98100000600000004</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="26">
+        <v>70</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0.98600000143051147</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0.98629999160766602</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0.9868999719619751</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0.9869999885559082</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0.98489999771118164</v>
+      </c>
+      <c r="U12" s="1">
+        <v>0.98589998483657837</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0.98449999094009399</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0.98309999704360962</v>
+      </c>
+      <c r="X12" s="41">
+        <v>0.97390002012252808</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A13" s="32"/>
+      <c r="B13" s="26">
+        <v>60</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.99089998000000001</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.99089998000000001</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.99089998000000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.99089998000000001</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.99089998000000001</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.99089998000000001</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.99049997300000003</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.98619997500000001</v>
+      </c>
+      <c r="K13" s="41">
+        <v>0.97289997299999997</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="26">
+        <v>60</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0.99089998006820679</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0.99089998006820679</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0.99089998006820679</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0.99049997329711914</v>
+      </c>
+      <c r="T13" s="1">
+        <v>0.98940002918243408</v>
+      </c>
+      <c r="U13" s="1">
+        <v>0.98890000581741333</v>
+      </c>
+      <c r="V13" s="1">
+        <v>0.98760002851486206</v>
+      </c>
+      <c r="W13" s="1">
+        <v>0.98119997978210449</v>
+      </c>
+      <c r="X13" s="41">
+        <v>0.97060000896453857</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A14" s="32"/>
+      <c r="B14" s="26">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.98900002200000003</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.98900002200000003</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.98900002200000003</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.98900002200000003</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.98900002200000003</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.98909997900000002</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.98760002899999999</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.97799998499999996</v>
+      </c>
+      <c r="K14" s="41">
+        <v>0.957499981</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="26">
+        <v>50</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0.98900002241134644</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0.98940002918243408</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0.98879998922348022</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0.98879998922348022</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0.98839998245239258</v>
+      </c>
+      <c r="U14" s="1">
+        <v>0.98720002174377441</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0.98100000619888306</v>
+      </c>
+      <c r="W14" s="1">
+        <v>0.97320002317428589</v>
+      </c>
+      <c r="X14" s="41">
+        <v>0.93470001220703125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A15" s="32"/>
+      <c r="B15" s="26">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.98729997899999999</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.98729997899999999</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.98729997899999999</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.98729997899999999</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.98729997899999999</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.98729997899999999</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.98589998499999998</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.98049998299999996</v>
+      </c>
+      <c r="K15" s="41">
+        <v>0.93000000699999996</v>
+      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="26">
+        <v>40</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0.98720002174377441</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0.98729997873306274</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0.98729997873306274</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0.98710000514984131</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0.98530000448226929</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0.98479998111724854</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0.9836999773979187</v>
+      </c>
+      <c r="W15" s="1">
+        <v>0.97939997911453247</v>
+      </c>
+      <c r="X15" s="41">
+        <v>0.96350002288818359</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A16" s="32"/>
+      <c r="B16" s="26">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.98530000399999995</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.98530000399999995</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.98530000399999995</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.98530000399999995</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.98530000399999995</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.98540002100000001</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.98460000800000003</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.98150002999999997</v>
+      </c>
+      <c r="K16" s="41">
+        <v>0.92280000399999995</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="26">
+        <v>30</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0.98530000448226929</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0.98509997129440308</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0.98449999094009399</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0.98420000076293945</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0.9846000075340271</v>
+      </c>
+      <c r="U16" s="1">
+        <v>0.98430001735687256</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0.98110002279281616</v>
+      </c>
+      <c r="W16" s="1">
+        <v>0.97920000553131104</v>
+      </c>
+      <c r="X16" s="41">
+        <v>0.92799997329711914</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A17" s="32"/>
+      <c r="B17" s="26">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.984000027</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.984000027</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.984000027</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.984000027</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.984000027</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.98439997400000001</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.98339998699999998</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.97689998099999997</v>
+      </c>
+      <c r="K17" s="41">
+        <v>0.85430002199999999</v>
+      </c>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="26">
+        <v>20</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0.98400002717971802</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0.98390001058578491</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0.98400002717971802</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0.98479998111724854</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0.98379999399185181</v>
+      </c>
+      <c r="U17" s="1">
+        <v>0.98269999027252197</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0.98229998350143433</v>
+      </c>
+      <c r="W17" s="1">
+        <v>0.97269999980926514</v>
+      </c>
+      <c r="X17" s="41">
+        <v>0.94279998540878296</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="33"/>
+      <c r="B18" s="27">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.97790002799999998</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.97790002799999998</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.97790002799999998</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.97790002799999998</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.97790002799999998</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.97799998499999996</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.97699999800000004</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.96590000399999998</v>
+      </c>
+      <c r="K18" s="41">
+        <v>0.81510001399999998</v>
+      </c>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="27">
+        <v>10</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0.97790002822875977</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0.97780001163482666</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0.97740000486373901</v>
+      </c>
+      <c r="S18" s="1">
+        <v>0.97680002450942993</v>
+      </c>
+      <c r="T18" s="1">
+        <v>0.97640001773834229</v>
+      </c>
+      <c r="U18" s="1">
+        <v>0.97630000114440918</v>
+      </c>
+      <c r="V18" s="1">
+        <v>0.97409999370574951</v>
+      </c>
+      <c r="W18" s="1">
+        <v>0.96619999408721924</v>
+      </c>
+      <c r="X18" s="41">
+        <v>0.94539999961853027</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A19" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="36"/>
+      <c r="C19" s="42">
+        <v>0.54232250041849006</v>
+      </c>
+      <c r="D19" s="43">
+        <v>0.54232250041849006</v>
+      </c>
+      <c r="E19" s="43">
+        <v>0.54232250041849006</v>
+      </c>
+      <c r="F19" s="43">
+        <v>0.54232250041849006</v>
+      </c>
+      <c r="G19" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="H19" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="I19" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="J19" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="K19" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="O19" s="36"/>
+      <c r="P19" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="Q19" s="43">
+        <v>0.80000318849590679</v>
+      </c>
+      <c r="R19" s="43">
+        <v>0.70000398561988342</v>
+      </c>
+      <c r="S19" s="43">
+        <v>0.6</v>
+      </c>
+      <c r="T19" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="U19" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="V19" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="W19" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="X19" s="44">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A20" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="45">
+        <v>2732988</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2732988</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2732988</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2732988</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2520612</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2018808</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1517004</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1015200</v>
+      </c>
+      <c r="K20" s="37">
+        <v>513396</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="O20" s="39"/>
+      <c r="P20" s="45">
+        <v>4534812</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>4033024</v>
+      </c>
+      <c r="R20" s="2">
+        <v>3531224</v>
+      </c>
+      <c r="S20" s="2">
+        <v>3029400</v>
+      </c>
+      <c r="T20" s="2">
+        <v>2527596</v>
+      </c>
+      <c r="U20" s="2">
+        <v>2025792</v>
+      </c>
+      <c r="V20" s="2">
+        <v>1523988</v>
+      </c>
+      <c r="W20" s="2">
+        <v>1022184</v>
+      </c>
+      <c r="X20" s="37">
+        <v>520380</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="40"/>
+      <c r="C21" s="46">
+        <f xml:space="preserve"> C20 / 1024^2</f>
+        <v>2.6063804626464844</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" ref="D21:K21" si="0" xml:space="preserve"> D20 / 1024^2</f>
+        <v>2.6063804626464844</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="0"/>
+        <v>2.6063804626464844</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="0"/>
+        <v>2.6063804626464844</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="0"/>
+        <v>2.4038429260253906</v>
+      </c>
+      <c r="H21" s="7">
+        <f t="shared" si="0"/>
+        <v>1.9252853393554688</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="0"/>
+        <v>1.4467277526855469</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="0"/>
+        <v>0.968170166015625</v>
+      </c>
+      <c r="K21" s="38">
+        <f t="shared" si="0"/>
+        <v>0.48961257934570313</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="O21" s="40"/>
+      <c r="P21" s="46">
+        <f xml:space="preserve"> P20 / 1024^2</f>
+        <v>4.3247337341308594</v>
+      </c>
+      <c r="Q21" s="7">
+        <f t="shared" ref="Q21" si="1" xml:space="preserve"> Q20 / 1024^2</f>
+        <v>3.84619140625</v>
+      </c>
+      <c r="R21" s="7">
+        <f t="shared" ref="R21" si="2" xml:space="preserve"> R20 / 1024^2</f>
+        <v>3.3676376342773438</v>
+      </c>
+      <c r="S21" s="7">
+        <f t="shared" ref="S21" si="3" xml:space="preserve"> S20 / 1024^2</f>
+        <v>2.8890609741210938</v>
+      </c>
+      <c r="T21" s="7">
+        <f t="shared" ref="T21" si="4" xml:space="preserve"> T20 / 1024^2</f>
+        <v>2.4105033874511719</v>
+      </c>
+      <c r="U21" s="7">
+        <f t="shared" ref="U21" si="5" xml:space="preserve"> U20 / 1024^2</f>
+        <v>1.93194580078125</v>
+      </c>
+      <c r="V21" s="7">
+        <f t="shared" ref="V21" si="6" xml:space="preserve"> V20 / 1024^2</f>
+        <v>1.4533882141113281</v>
+      </c>
+      <c r="W21" s="7">
+        <f t="shared" ref="W21" si="7" xml:space="preserve"> W20 / 1024^2</f>
+        <v>0.97483062744140625</v>
+      </c>
+      <c r="X21" s="38">
+        <f t="shared" ref="X21" si="8" xml:space="preserve"> X20 / 1024^2</f>
+        <v>0.49627304077148438</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+    </row>
+    <row r="25" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+    </row>
+    <row r="26" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="35"/>
+      <c r="T27" s="35"/>
+      <c r="U27" s="35"/>
+      <c r="V27" s="35"/>
+      <c r="W27" s="35"/>
+      <c r="X27" s="36"/>
+    </row>
+    <row r="28" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="6">
+        <v>10</v>
+      </c>
+      <c r="D28" s="47">
+        <v>20</v>
+      </c>
+      <c r="E28" s="47">
+        <v>30</v>
+      </c>
+      <c r="F28" s="47">
+        <v>40</v>
+      </c>
+      <c r="G28" s="47">
+        <v>50</v>
+      </c>
+      <c r="H28" s="47">
+        <v>60</v>
+      </c>
+      <c r="I28" s="47">
+        <v>70</v>
+      </c>
+      <c r="J28" s="47">
+        <v>80</v>
+      </c>
+      <c r="K28" s="27">
+        <v>90</v>
+      </c>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q28" s="47">
+        <v>20</v>
+      </c>
+      <c r="R28" s="47">
+        <v>30</v>
+      </c>
+      <c r="S28" s="47">
+        <v>40</v>
+      </c>
+      <c r="T28" s="47">
+        <v>50</v>
+      </c>
+      <c r="U28" s="47">
+        <v>60</v>
+      </c>
+      <c r="V28" s="47">
+        <v>70</v>
+      </c>
+      <c r="W28" s="47">
+        <v>80</v>
+      </c>
+      <c r="X28" s="27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A29" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="25">
+        <v>100</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="K29" s="41">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="N29" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="O29" s="25">
+        <v>100</v>
+      </c>
+      <c r="P29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="R29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="T29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="U29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="V29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="W29" s="1">
+        <v>0.99180001020431519</v>
+      </c>
+      <c r="X29" s="41">
+        <v>0.99180001020431519</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A30" s="32"/>
+      <c r="B30" s="26">
+        <v>90</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.98830002546310425</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.98839998245239258</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.98849999904632568</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.98869997262954712</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.98909997940063477</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.9901999831199646</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.99049997329711914</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0.99119997024536133</v>
+      </c>
+      <c r="K30" s="41">
+        <v>0.99070000648498535</v>
+      </c>
+      <c r="N30" s="32"/>
+      <c r="O30" s="26">
+        <v>90</v>
+      </c>
+      <c r="P30" s="1">
+        <v>0.98830002546310425</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>0.98839998245239258</v>
+      </c>
+      <c r="R30" s="1">
+        <v>0.98849999904632568</v>
+      </c>
+      <c r="S30" s="1">
+        <v>0.98869997262954712</v>
+      </c>
+      <c r="T30" s="1">
+        <v>0.98909997940063477</v>
+      </c>
+      <c r="U30" s="1">
+        <v>0.9901999831199646</v>
+      </c>
+      <c r="V30" s="1">
+        <v>0.99049997329711914</v>
+      </c>
+      <c r="W30" s="1">
+        <v>0.99119997024536133</v>
+      </c>
+      <c r="X30" s="41">
+        <v>0.99070000648498535</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A31" s="32"/>
+      <c r="B31" s="26">
+        <v>80</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.98960000276565552</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.98930001258850098</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.98919999599456787</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.98869997262954712</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.98750001192092896</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.98729997873306274</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.9879000186920166</v>
+      </c>
+      <c r="K31" s="41">
+        <v>0.98530000448226929</v>
+      </c>
+      <c r="N31" s="32"/>
+      <c r="O31" s="26">
+        <v>80</v>
+      </c>
+      <c r="P31" s="1">
+        <v>0.98960000276565552</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="R31" s="1">
+        <v>0.98930001258850098</v>
+      </c>
+      <c r="S31" s="1">
+        <v>0.98940002918243408</v>
+      </c>
+      <c r="T31" s="1">
+        <v>0.98869997262954712</v>
+      </c>
+      <c r="U31" s="1">
+        <v>0.98940002918243408</v>
+      </c>
+      <c r="V31" s="1">
+        <v>0.9878000020980835</v>
+      </c>
+      <c r="W31" s="1">
+        <v>0.9868999719619751</v>
+      </c>
+      <c r="X31" s="41">
+        <v>0.98549997806549072</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A32" s="32"/>
+      <c r="B32" s="26">
+        <v>70</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.98600000143051147</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.98610001802444458</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.98650002479553223</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0.98629999160766602</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.98559999465942383</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0.98509997129440308</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0.98470002412796021</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0.98439997434616089</v>
+      </c>
+      <c r="K32" s="41">
+        <v>0.97970002889633179</v>
+      </c>
+      <c r="N32" s="32"/>
+      <c r="O32" s="26">
+        <v>70</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0.98600000143051147</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>0.98619997501373291</v>
+      </c>
+      <c r="R32" s="1">
+        <v>0.9868999719619751</v>
+      </c>
+      <c r="S32" s="1">
+        <v>0.98650002479553223</v>
+      </c>
+      <c r="T32" s="1">
+        <v>0.98509997129440308</v>
+      </c>
+      <c r="U32" s="1">
+        <v>0.98600000143051147</v>
+      </c>
+      <c r="V32" s="1">
+        <v>0.98449999094009399</v>
+      </c>
+      <c r="W32" s="1">
+        <v>0.98320001363754272</v>
+      </c>
+      <c r="X32" s="41">
+        <v>0.97909998893737793</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A33" s="32"/>
+      <c r="B33" s="26">
+        <v>60</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.99089998006820679</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.99080002307891846</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.99059998989105225</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.99070000648498535</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.98989999294281006</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0.98729997873306274</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0.98519998788833618</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.982200026512146</v>
+      </c>
+      <c r="K33" s="41">
+        <v>0.96410000324249268</v>
+      </c>
+      <c r="N33" s="32"/>
+      <c r="O33" s="26">
+        <v>60</v>
+      </c>
+      <c r="P33" s="1">
+        <v>0.99089998006820679</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>0.991100013256073</v>
+      </c>
+      <c r="R33" s="1">
+        <v>0.99099999666213989</v>
+      </c>
+      <c r="S33" s="1">
+        <v>0.99040001630783081</v>
+      </c>
+      <c r="T33" s="1">
+        <v>0.98940002918243408</v>
+      </c>
+      <c r="U33" s="1">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="V33" s="1">
+        <v>0.98650002479553223</v>
+      </c>
+      <c r="W33" s="1">
+        <v>0.9814000129699707</v>
+      </c>
+      <c r="X33" s="41">
+        <v>0.97140002250671387</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A34" s="32"/>
+      <c r="B34" s="26">
+        <v>50</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.98900002241134644</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.98900002241134644</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.98900002241134644</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.98849999904632568</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.98820000886917114</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0.98669999837875366</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0.98030000925064087</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0.97259998321533203</v>
+      </c>
+      <c r="K34" s="41">
+        <v>0.94330000877380371</v>
+      </c>
+      <c r="N34" s="32"/>
+      <c r="O34" s="26">
+        <v>50</v>
+      </c>
+      <c r="P34" s="1">
+        <v>0.98900002241134644</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>0.98940002918243408</v>
+      </c>
+      <c r="R34" s="1">
+        <v>0.98799997568130493</v>
+      </c>
+      <c r="S34" s="1">
+        <v>0.98869997262954712</v>
+      </c>
+      <c r="T34" s="1">
+        <v>0.98760002851486206</v>
+      </c>
+      <c r="U34" s="1">
+        <v>0.98519998788833618</v>
+      </c>
+      <c r="V34" s="1">
+        <v>0.97899997234344482</v>
+      </c>
+      <c r="W34" s="1">
+        <v>0.95080000162124634</v>
+      </c>
+      <c r="X34" s="41">
+        <v>0.92040002346038818</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A35" s="32"/>
+      <c r="B35" s="26">
+        <v>40</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.98729997873306274</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.98739999532699585</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.98720002174377441</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.98729997873306274</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.98760002851486206</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.98650002479553223</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0.97899997234344482</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0.97649997472763062</v>
+      </c>
+      <c r="K35" s="41">
+        <v>0.90829998254776001</v>
+      </c>
+      <c r="N35" s="32"/>
+      <c r="O35" s="26">
+        <v>40</v>
+      </c>
+      <c r="P35" s="1">
+        <v>0.98720002174377441</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>0.98710000514984131</v>
+      </c>
+      <c r="R35" s="1">
+        <v>0.98729997873306274</v>
+      </c>
+      <c r="S35" s="1">
+        <v>0.98669999837875366</v>
+      </c>
+      <c r="T35" s="1">
+        <v>0.98509997129440308</v>
+      </c>
+      <c r="U35" s="1">
+        <v>0.98320001363754272</v>
+      </c>
+      <c r="V35" s="1">
+        <v>0.98119997978210449</v>
+      </c>
+      <c r="W35" s="1">
+        <v>0.9692000150680542</v>
+      </c>
+      <c r="X35" s="41">
+        <v>0.91600000858306885</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A36" s="32"/>
+      <c r="B36" s="26">
+        <v>30</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.98530000448226929</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.98540002107620239</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.98570001125335693</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0.98580002784729004</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0.98559999465942383</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.98619997501373291</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0.98079997301101685</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0.97960001230239868</v>
+      </c>
+      <c r="K36" s="41">
+        <v>0.91610002517700195</v>
+      </c>
+      <c r="N36" s="32"/>
+      <c r="O36" s="26">
+        <v>30</v>
+      </c>
+      <c r="P36" s="1">
+        <v>0.98530000448226929</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>0.98530000448226929</v>
+      </c>
+      <c r="R36" s="1">
+        <v>0.9846000075340271</v>
+      </c>
+      <c r="S36" s="1">
+        <v>0.9846000075340271</v>
+      </c>
+      <c r="T36" s="1">
+        <v>0.98479998111724854</v>
+      </c>
+      <c r="U36" s="1">
+        <v>0.98299998044967651</v>
+      </c>
+      <c r="V36" s="1">
+        <v>0.97879999876022339</v>
+      </c>
+      <c r="W36" s="1">
+        <v>0.97020000219345093</v>
+      </c>
+      <c r="X36" s="41">
+        <v>0.87489998340606689</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A37" s="32"/>
+      <c r="B37" s="26">
+        <v>20</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.98400002717971802</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.98400002717971802</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.98420000076293945</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.98390001058578491</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.98269999027252197</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.98210000991821289</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0.97920000553131104</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0.96480000019073486</v>
+      </c>
+      <c r="K37" s="41">
+        <v>0.85000002384185791</v>
+      </c>
+      <c r="N37" s="32"/>
+      <c r="O37" s="26">
+        <v>20</v>
+      </c>
+      <c r="P37" s="1">
+        <v>0.98400002717971802</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0.9836999773979187</v>
+      </c>
+      <c r="R37" s="1">
+        <v>0.98470002412796021</v>
+      </c>
+      <c r="S37" s="1">
+        <v>0.98479998111724854</v>
+      </c>
+      <c r="T37" s="1">
+        <v>0.98400002717971802</v>
+      </c>
+      <c r="U37" s="1">
+        <v>0.98309999704360962</v>
+      </c>
+      <c r="V37" s="1">
+        <v>0.97780001163482666</v>
+      </c>
+      <c r="W37" s="1">
+        <v>0.96170002222061157</v>
+      </c>
+      <c r="X37" s="41">
+        <v>0.7896999716758728</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="33"/>
+      <c r="B38" s="27">
+        <v>10</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.97780001163482666</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.9779999852180481</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.97839999198913574</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.97710001468658447</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.97680002450942993</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0.97549998760223389</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0.97170001268386841</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0.9538000226020813</v>
+      </c>
+      <c r="K38" s="41">
+        <v>0.86529999971389771</v>
+      </c>
+      <c r="N38" s="33"/>
+      <c r="O38" s="27">
+        <v>10</v>
+      </c>
+      <c r="P38" s="1">
+        <v>0.97790002822875977</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>0.97769999504089355</v>
+      </c>
+      <c r="R38" s="1">
+        <v>0.97710001468658447</v>
+      </c>
+      <c r="S38" s="1">
+        <v>0.97659999132156372</v>
+      </c>
+      <c r="T38" s="1">
+        <v>0.97610002756118774</v>
+      </c>
+      <c r="U38" s="1">
+        <v>0.97460001707077026</v>
+      </c>
+      <c r="V38" s="1">
+        <v>0.96789997816085815</v>
+      </c>
+      <c r="W38" s="1">
+        <v>0.94690001010894775</v>
+      </c>
+      <c r="X38" s="41">
+        <v>0.75180000066757202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A39" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="36"/>
+      <c r="C39" s="42">
+        <v>0.53121138930737899</v>
+      </c>
+      <c r="D39" s="43">
+        <v>0.51137735051932631</v>
+      </c>
+      <c r="E39" s="43">
+        <v>0.48198579525073543</v>
+      </c>
+      <c r="F39" s="43">
+        <v>0.44343847398585901</v>
+      </c>
+      <c r="G39" s="43">
+        <v>0.39455404899123958</v>
+      </c>
+      <c r="H39" s="43">
+        <v>0.33647798742138357</v>
+      </c>
+      <c r="I39" s="43">
+        <v>0.26858454695458778</v>
+      </c>
+      <c r="J39" s="43">
+        <v>0.1901411706562722</v>
+      </c>
+      <c r="K39" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="N39" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="O39" s="36"/>
+      <c r="P39" s="42">
+        <v>0.9</v>
+      </c>
+      <c r="Q39" s="43">
+        <v>0.8</v>
+      </c>
+      <c r="R39" s="43">
+        <v>0.7</v>
+      </c>
+      <c r="S39" s="43">
+        <v>0.6</v>
+      </c>
+      <c r="T39" s="43">
+        <v>0.50000079712397671</v>
+      </c>
+      <c r="U39" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="V39" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="W39" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="X39" s="44">
+        <v>0.10000079712397671</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A40" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="39"/>
+      <c r="C40" s="45">
+        <v>2677232</v>
+      </c>
+      <c r="D40" s="2">
+        <v>2577704</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2430216</v>
+      </c>
+      <c r="F40" s="2">
+        <v>2236784</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1991480</v>
+      </c>
+      <c r="H40" s="2">
+        <v>1700052</v>
+      </c>
+      <c r="I40" s="2">
+        <v>1359360</v>
+      </c>
+      <c r="J40" s="2">
+        <v>965728</v>
+      </c>
+      <c r="K40" s="37">
+        <v>513396</v>
+      </c>
+      <c r="N40" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="O40" s="39"/>
+      <c r="P40" s="45">
+        <v>4534812</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>4033008</v>
+      </c>
+      <c r="R40" s="2">
+        <v>3531204</v>
+      </c>
+      <c r="S40" s="2">
+        <v>3029400</v>
+      </c>
+      <c r="T40" s="2">
+        <v>2527600</v>
+      </c>
+      <c r="U40" s="2">
+        <v>2025792</v>
+      </c>
+      <c r="V40" s="2">
+        <v>1523988</v>
+      </c>
+      <c r="W40" s="2">
+        <v>1022184</v>
+      </c>
+      <c r="X40" s="37">
+        <v>520384</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="40"/>
+      <c r="C41" s="46">
+        <f xml:space="preserve"> C40 / 1024^2</f>
+        <v>2.5532073974609375</v>
+      </c>
+      <c r="D41" s="7">
+        <f t="shared" ref="D41" si="9" xml:space="preserve"> D40 / 1024^2</f>
+        <v>2.4582901000976563</v>
+      </c>
+      <c r="E41" s="7">
+        <f t="shared" ref="E41" si="10" xml:space="preserve"> E40 / 1024^2</f>
+        <v>2.3176345825195313</v>
+      </c>
+      <c r="F41" s="7">
+        <f t="shared" ref="F41" si="11" xml:space="preserve"> F40 / 1024^2</f>
+        <v>2.1331634521484375</v>
+      </c>
+      <c r="G41" s="7">
+        <f t="shared" ref="G41" si="12" xml:space="preserve"> G40 / 1024^2</f>
+        <v>1.8992233276367188</v>
+      </c>
+      <c r="H41" s="7">
+        <f t="shared" ref="H41" si="13" xml:space="preserve"> H40 / 1024^2</f>
+        <v>1.6212959289550781</v>
+      </c>
+      <c r="I41" s="7">
+        <f t="shared" ref="I41" si="14" xml:space="preserve"> I40 / 1024^2</f>
+        <v>1.29638671875</v>
+      </c>
+      <c r="J41" s="7">
+        <f t="shared" ref="J41" si="15" xml:space="preserve"> J40 / 1024^2</f>
+        <v>0.920989990234375</v>
+      </c>
+      <c r="K41" s="38">
+        <f t="shared" ref="K41" si="16" xml:space="preserve"> K40 / 1024^2</f>
+        <v>0.48961257934570313</v>
+      </c>
+      <c r="N41" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="O41" s="40"/>
+      <c r="P41" s="46">
+        <f xml:space="preserve"> P40 / 1024^2</f>
+        <v>4.3247337341308594</v>
+      </c>
+      <c r="Q41" s="7">
+        <f t="shared" ref="Q41" si="17" xml:space="preserve"> Q40 / 1024^2</f>
+        <v>3.8461761474609375</v>
+      </c>
+      <c r="R41" s="7">
+        <f t="shared" ref="R41" si="18" xml:space="preserve"> R40 / 1024^2</f>
+        <v>3.3676185607910156</v>
+      </c>
+      <c r="S41" s="7">
+        <f t="shared" ref="S41" si="19" xml:space="preserve"> S40 / 1024^2</f>
+        <v>2.8890609741210938</v>
+      </c>
+      <c r="T41" s="7">
+        <f t="shared" ref="T41" si="20" xml:space="preserve"> T40 / 1024^2</f>
+        <v>2.4105072021484375</v>
+      </c>
+      <c r="U41" s="7">
+        <f t="shared" ref="U41" si="21" xml:space="preserve"> U40 / 1024^2</f>
+        <v>1.93194580078125</v>
+      </c>
+      <c r="V41" s="7">
+        <f t="shared" ref="V41" si="22" xml:space="preserve"> V40 / 1024^2</f>
+        <v>1.4533882141113281</v>
+      </c>
+      <c r="W41" s="7">
+        <f t="shared" ref="W41" si="23" xml:space="preserve"> W40 / 1024^2</f>
+        <v>0.97483062744140625</v>
+      </c>
+      <c r="X41" s="38">
+        <f t="shared" ref="X41" si="24" xml:space="preserve"> X40 / 1024^2</f>
+        <v>0.49627685546875</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="P27:X27"/>
+    <mergeCell ref="N29:N38"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C27:K27"/>
+    <mergeCell ref="A29:A38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="P7:X7"/>
+    <mergeCell ref="N9:N18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="A9:A18"/>
+    <mergeCell ref="C7:K7"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A19:B19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More result table changes.
</commit_message>
<xml_diff>
--- a/experiments/results/results.xlsx
+++ b/experiments/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VU\Code\SubFlow\experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25B6B47-7D4A-419C-962F-8927B20475F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7CD9AE-6883-4461-9527-D36BDB6D3804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline" sheetId="1" r:id="rId1"/>
@@ -767,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -3335,8 +3335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6C6186-6B13-4104-96F4-C771BEA453CD}">
   <dimension ref="A3:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AD40" sqref="AD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4674,15 +4674,33 @@
       <c r="O29" s="25">
         <v>100</v>
       </c>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="18"/>
-      <c r="T29" s="18"/>
-      <c r="U29" s="18"/>
-      <c r="V29" s="18"/>
-      <c r="W29" s="18"/>
-      <c r="X29" s="19"/>
+      <c r="P29" s="18">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="Q29" s="18">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="R29" s="18">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="S29" s="18">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="T29" s="18">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="U29" s="18">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="V29" s="18">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="W29" s="18">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="X29" s="19">
+        <v>0.98949998617172241</v>
+      </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" s="32"/>
@@ -4720,15 +4738,33 @@
       <c r="O30" s="26">
         <v>90</v>
       </c>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
-      <c r="U30" s="18"/>
-      <c r="V30" s="18"/>
-      <c r="W30" s="18"/>
-      <c r="X30" s="19"/>
+      <c r="P30" s="18">
+        <v>0.98589998483657837</v>
+      </c>
+      <c r="Q30" s="18">
+        <v>0.98629999160766602</v>
+      </c>
+      <c r="R30" s="18">
+        <v>0.98650002479553223</v>
+      </c>
+      <c r="S30" s="18">
+        <v>0.98659998178482056</v>
+      </c>
+      <c r="T30" s="18">
+        <v>0.98869997262954712</v>
+      </c>
+      <c r="U30" s="18">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="V30" s="18">
+        <v>0.98879998922348022</v>
+      </c>
+      <c r="W30" s="18">
+        <v>0.98849999904632568</v>
+      </c>
+      <c r="X30" s="19">
+        <v>0.98750001192092896</v>
+      </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" s="32"/>
@@ -4766,15 +4802,33 @@
       <c r="O31" s="26">
         <v>80</v>
       </c>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="18"/>
-      <c r="U31" s="18"/>
-      <c r="V31" s="18"/>
-      <c r="W31" s="18"/>
-      <c r="X31" s="19"/>
+      <c r="P31" s="18">
+        <v>0.99049997329711914</v>
+      </c>
+      <c r="Q31" s="18">
+        <v>0.99010002613067627</v>
+      </c>
+      <c r="R31" s="18">
+        <v>0.98970001935958862</v>
+      </c>
+      <c r="S31" s="18">
+        <v>0.98949998617172241</v>
+      </c>
+      <c r="T31" s="18">
+        <v>0.98979997634887695</v>
+      </c>
+      <c r="U31" s="18">
+        <v>0.98919999599456787</v>
+      </c>
+      <c r="V31" s="18">
+        <v>0.98940002918243408</v>
+      </c>
+      <c r="W31" s="18">
+        <v>0.98909997940063477</v>
+      </c>
+      <c r="X31" s="19">
+        <v>0.98559999465942383</v>
+      </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A32" s="32"/>
@@ -4812,15 +4866,33 @@
       <c r="O32" s="26">
         <v>70</v>
       </c>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="19"/>
+      <c r="P32" s="18">
+        <v>0.9878000020980835</v>
+      </c>
+      <c r="Q32" s="18">
+        <v>0.98750001192092896</v>
+      </c>
+      <c r="R32" s="18">
+        <v>0.98729997873306274</v>
+      </c>
+      <c r="S32" s="18">
+        <v>0.98739999532699585</v>
+      </c>
+      <c r="T32" s="18">
+        <v>0.9869999885559082</v>
+      </c>
+      <c r="U32" s="18">
+        <v>0.98619997501373291</v>
+      </c>
+      <c r="V32" s="18">
+        <v>0.98559999465942383</v>
+      </c>
+      <c r="W32" s="18">
+        <v>0.98559999465942383</v>
+      </c>
+      <c r="X32" s="19">
+        <v>0.97890001535415649</v>
+      </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33" s="32"/>
@@ -4858,15 +4930,33 @@
       <c r="O33" s="26">
         <v>60</v>
       </c>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
-      <c r="U33" s="18"/>
-      <c r="V33" s="18"/>
-      <c r="W33" s="18"/>
-      <c r="X33" s="19"/>
+      <c r="P33" s="18">
+        <v>0.98750001192092896</v>
+      </c>
+      <c r="Q33" s="18">
+        <v>0.98799997568130493</v>
+      </c>
+      <c r="R33" s="18">
+        <v>0.98729997873306274</v>
+      </c>
+      <c r="S33" s="18">
+        <v>0.98760002851486206</v>
+      </c>
+      <c r="T33" s="18">
+        <v>0.98680001497268677</v>
+      </c>
+      <c r="U33" s="18">
+        <v>0.9868999719619751</v>
+      </c>
+      <c r="V33" s="18">
+        <v>0.98360002040863037</v>
+      </c>
+      <c r="W33" s="18">
+        <v>0.98070001602172852</v>
+      </c>
+      <c r="X33" s="19">
+        <v>0.97710001468658447</v>
+      </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" s="32"/>
@@ -4904,15 +4994,33 @@
       <c r="O34" s="26">
         <v>50</v>
       </c>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
-      <c r="T34" s="18"/>
-      <c r="U34" s="18"/>
-      <c r="V34" s="18"/>
-      <c r="W34" s="18"/>
-      <c r="X34" s="19"/>
+      <c r="P34" s="18">
+        <v>0.98799997568130493</v>
+      </c>
+      <c r="Q34" s="18">
+        <v>0.9878000020980835</v>
+      </c>
+      <c r="R34" s="18">
+        <v>0.98750001192092896</v>
+      </c>
+      <c r="S34" s="18">
+        <v>0.98760002851486206</v>
+      </c>
+      <c r="T34" s="18">
+        <v>0.98710000514984131</v>
+      </c>
+      <c r="U34" s="18">
+        <v>0.98720002174377441</v>
+      </c>
+      <c r="V34" s="18">
+        <v>0.98619997501373291</v>
+      </c>
+      <c r="W34" s="18">
+        <v>0.98110002279281616</v>
+      </c>
+      <c r="X34" s="19">
+        <v>0.97549998760223389</v>
+      </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" s="32"/>
@@ -4950,15 +5058,33 @@
       <c r="O35" s="26">
         <v>40</v>
       </c>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
-      <c r="T35" s="18"/>
-      <c r="U35" s="18"/>
-      <c r="V35" s="18"/>
-      <c r="W35" s="18"/>
-      <c r="X35" s="19"/>
+      <c r="P35" s="18">
+        <v>0.98530000448226929</v>
+      </c>
+      <c r="Q35" s="18">
+        <v>0.98500001430511475</v>
+      </c>
+      <c r="R35" s="18">
+        <v>0.98540002107620239</v>
+      </c>
+      <c r="S35" s="18">
+        <v>0.98519998788833618</v>
+      </c>
+      <c r="T35" s="18">
+        <v>0.98489999771118164</v>
+      </c>
+      <c r="U35" s="18">
+        <v>0.98400002717971802</v>
+      </c>
+      <c r="V35" s="18">
+        <v>0.9836999773979187</v>
+      </c>
+      <c r="W35" s="18">
+        <v>0.98379999399185181</v>
+      </c>
+      <c r="X35" s="19">
+        <v>0.97189998626708984</v>
+      </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A36" s="32"/>
@@ -4996,15 +5122,33 @@
       <c r="O36" s="26">
         <v>30</v>
       </c>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
-      <c r="T36" s="18"/>
-      <c r="U36" s="18"/>
-      <c r="V36" s="18"/>
-      <c r="W36" s="18"/>
-      <c r="X36" s="19"/>
+      <c r="P36" s="18">
+        <v>0.98629999160766602</v>
+      </c>
+      <c r="Q36" s="18">
+        <v>0.98589998483657837</v>
+      </c>
+      <c r="R36" s="18">
+        <v>0.98610001802444458</v>
+      </c>
+      <c r="S36" s="18">
+        <v>0.98629999160766602</v>
+      </c>
+      <c r="T36" s="18">
+        <v>0.98610001802444458</v>
+      </c>
+      <c r="U36" s="18">
+        <v>0.98619997501373291</v>
+      </c>
+      <c r="V36" s="18">
+        <v>0.98259997367858887</v>
+      </c>
+      <c r="W36" s="18">
+        <v>0.98229998350143433</v>
+      </c>
+      <c r="X36" s="19">
+        <v>0.97839999198913574</v>
+      </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37" s="32"/>
@@ -5042,15 +5186,33 @@
       <c r="O37" s="26">
         <v>20</v>
       </c>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
-      <c r="T37" s="18"/>
-      <c r="U37" s="18"/>
-      <c r="V37" s="18"/>
-      <c r="W37" s="18"/>
-      <c r="X37" s="19"/>
+      <c r="P37" s="18">
+        <v>0.98070001602172852</v>
+      </c>
+      <c r="Q37" s="18">
+        <v>0.98059999942779541</v>
+      </c>
+      <c r="R37" s="18">
+        <v>0.98079997301101685</v>
+      </c>
+      <c r="S37" s="18">
+        <v>0.98009997606277466</v>
+      </c>
+      <c r="T37" s="18">
+        <v>0.98019999265670776</v>
+      </c>
+      <c r="U37" s="18">
+        <v>0.97930002212524414</v>
+      </c>
+      <c r="V37" s="18">
+        <v>0.9779999852180481</v>
+      </c>
+      <c r="W37" s="18">
+        <v>0.97939997911453247</v>
+      </c>
+      <c r="X37" s="19">
+        <v>0.97009998559951782</v>
+      </c>
     </row>
     <row r="38" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="33"/>
@@ -5088,15 +5250,33 @@
       <c r="O38" s="27">
         <v>10</v>
       </c>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="18"/>
-      <c r="U38" s="18"/>
-      <c r="V38" s="18"/>
-      <c r="W38" s="18"/>
-      <c r="X38" s="19"/>
+      <c r="P38" s="18">
+        <v>0.97469997406005859</v>
+      </c>
+      <c r="Q38" s="18">
+        <v>0.9747999906539917</v>
+      </c>
+      <c r="R38" s="18">
+        <v>0.97460001707077026</v>
+      </c>
+      <c r="S38" s="18">
+        <v>0.9747999906539917</v>
+      </c>
+      <c r="T38" s="18">
+        <v>0.97390002012252808</v>
+      </c>
+      <c r="U38" s="18">
+        <v>0.97369998693466187</v>
+      </c>
+      <c r="V38" s="18">
+        <v>0.97219997644424438</v>
+      </c>
+      <c r="W38" s="18">
+        <v>0.96649998426437378</v>
+      </c>
+      <c r="X38" s="19">
+        <v>0.95770001411437988</v>
+      </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" s="34" t="s">
@@ -5134,15 +5314,33 @@
         <v>27</v>
       </c>
       <c r="O39" s="36"/>
-      <c r="P39" s="41"/>
-      <c r="Q39" s="42"/>
-      <c r="R39" s="42"/>
-      <c r="S39" s="42"/>
-      <c r="T39" s="42"/>
-      <c r="U39" s="42"/>
-      <c r="V39" s="42"/>
-      <c r="W39" s="42"/>
-      <c r="X39" s="43"/>
+      <c r="P39" s="41">
+        <v>0.9</v>
+      </c>
+      <c r="Q39" s="42">
+        <v>0.8</v>
+      </c>
+      <c r="R39" s="42">
+        <v>0.7</v>
+      </c>
+      <c r="S39" s="42">
+        <v>0.6</v>
+      </c>
+      <c r="T39" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="U39" s="42">
+        <v>0.4</v>
+      </c>
+      <c r="V39" s="42">
+        <v>0.3</v>
+      </c>
+      <c r="W39" s="42">
+        <v>0.2</v>
+      </c>
+      <c r="X39" s="43">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" s="47" t="s">
@@ -5180,15 +5378,33 @@
         <v>25</v>
       </c>
       <c r="O40" s="39"/>
-      <c r="P40" s="44"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
-      <c r="W40" s="2"/>
-      <c r="X40" s="37"/>
+      <c r="P40" s="44">
+        <v>4534812</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>4033008</v>
+      </c>
+      <c r="R40" s="2">
+        <v>3531204</v>
+      </c>
+      <c r="S40" s="2">
+        <v>3029400</v>
+      </c>
+      <c r="T40" s="2">
+        <v>2527596</v>
+      </c>
+      <c r="U40" s="2">
+        <v>2025792</v>
+      </c>
+      <c r="V40" s="2">
+        <v>1523988</v>
+      </c>
+      <c r="W40" s="2">
+        <v>1022184</v>
+      </c>
+      <c r="X40" s="37">
+        <v>520380</v>
+      </c>
     </row>
     <row r="41" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="48" t="s">
@@ -5237,39 +5453,39 @@
       <c r="O41" s="40"/>
       <c r="P41" s="45">
         <f xml:space="preserve"> P40 / 1024^2</f>
-        <v>0</v>
+        <v>4.3247337341308594</v>
       </c>
       <c r="Q41" s="7">
         <f t="shared" ref="Q41:X41" si="3" xml:space="preserve"> Q40 / 1024^2</f>
-        <v>0</v>
+        <v>3.8461761474609375</v>
       </c>
       <c r="R41" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.3676185607910156</v>
       </c>
       <c r="S41" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.8890609741210938</v>
       </c>
       <c r="T41" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.4105033874511719</v>
       </c>
       <c r="U41" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.93194580078125</v>
       </c>
       <c r="V41" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.4533882141113281</v>
       </c>
       <c r="W41" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.97483062744140625</v>
       </c>
       <c r="X41" s="38">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.49627304077148438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>